<commit_message>
code done,will fix bug
</commit_message>
<xml_diff>
--- a/app/project/MDK_V5/AT32F415RBT7_WorkBench_analysis.xlsx
+++ b/app/project/MDK_V5/AT32F415RBT7_WorkBench_analysis.xlsx
@@ -15,12 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t>AT32F415RBT7_WorkBench</t>
   </si>
   <si>
-    <t>lto-llvm-2a85c4.o</t>
+    <t>lto-llvm-5b4722.o</t>
   </si>
   <si>
     <t>startup_at32f415.o</t>
@@ -32,6 +32,9 @@
     <t>stdout.o</t>
   </si>
   <si>
+    <t>printfa.o</t>
+  </si>
+  <si>
     <t>mf_w.l</t>
   </si>
   <si>
@@ -50,19 +53,40 @@
     <t>fadd.o</t>
   </si>
   <si>
+    <t>fdiv.o</t>
+  </si>
+  <si>
     <t>fepilogue.o</t>
   </si>
   <si>
     <t>fmul.o</t>
   </si>
   <si>
+    <t>uldiv.o</t>
+  </si>
+  <si>
     <t>dfixi.o</t>
   </si>
   <si>
+    <t>ffixi.o</t>
+  </si>
+  <si>
+    <t>dfixui.o</t>
+  </si>
+  <si>
+    <t>dfixul.o</t>
+  </si>
+  <si>
+    <t>cdrcmple.o</t>
+  </si>
+  <si>
+    <t>uidiv.o</t>
+  </si>
+  <si>
     <t>ffixui.o</t>
   </si>
   <si>
-    <t>puts.o</t>
+    <t>f2d.o</t>
   </si>
   <si>
     <t>memseta.o</t>
@@ -75,6 +99,9 @@
   </si>
   <si>
     <t>init.o</t>
+  </si>
+  <si>
+    <t>dflti.o</t>
   </si>
   <si>
     <t>llushr.o</t>
@@ -233,11 +260,11 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>ram_percent!$A$3:$A$35</c:f>
+              <c:f>ram_percent!$A$3:$A$44</c:f>
               <c:strCache>
-                <c:ptCount val="33"/>
+                <c:ptCount val="42"/>
                 <c:pt idx="0">
-                  <c:v>lto-llvm-2a85c4.o</c:v>
+                  <c:v>lto-llvm-5b4722.o</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>startup_at32f415.o</c:v>
@@ -248,7 +275,7 @@
                 <c:pt idx="3">
                   <c:v>stdout.o</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="41">
                   <c:v>Totals</c:v>
                 </c:pt>
               </c:strCache>
@@ -256,23 +283,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ram_percent!$B$3:$B$35</c:f>
+              <c:f>ram_percent!$B$3:$B$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="42"/>
                 <c:pt idx="0">
-                  <c:v>85.74585723876953</c:v>
+                  <c:v>83.91521453857422</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.14364624023438</c:v>
+                  <c:v>15.9601001739502</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.05524861812591553</c:v>
+                  <c:v>0.06234414130449295</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.05524861812591553</c:v>
-                </c:pt>
-                <c:pt idx="32">
+                  <c:v>0.06234414130449295</c:v>
+                </c:pt>
+                <c:pt idx="41">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -340,106 +367,133 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>flash_percent!$A$3:$A$35</c:f>
+              <c:f>flash_percent!$A$3:$A$44</c:f>
               <c:strCache>
-                <c:ptCount val="33"/>
+                <c:ptCount val="42"/>
                 <c:pt idx="0">
-                  <c:v>lto-llvm-2a85c4.o</c:v>
+                  <c:v>lto-llvm-5b4722.o</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>mc_w.l</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>printfa.o</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>mf_w.l</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>startup_at32f415.o</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>dadd.o</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>mc_w.l</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>dmul.o</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>ddiv.o</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>depilogue.o</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>fadd.o</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
+                  <c:v>fdiv.o</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>fepilogue.o</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>fmul.o</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
+                  <c:v>uldiv.o</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>dfixi.o</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
+                  <c:v>ffixi.o</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>dfixui.o</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>dfixul.o</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>cdrcmple.o</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>uidiv.o</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>ffixui.o</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>puts.o</c:v>
-                </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="21">
+                  <c:v>f2d.o</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>memseta.o</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="23">
                   <c:v>memcpya.o</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="24">
                   <c:v>llsshr.o</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="25">
                   <c:v>init.o</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="26">
+                  <c:v>dflti.o</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>llushr.o</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="28">
                   <c:v>llshl.o</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="29">
                   <c:v>handlers.o</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="30">
                   <c:v>fcmplt.o</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="31">
                   <c:v>fcmple.o</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="32">
                   <c:v>fcmpgt.o</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="33">
                   <c:v>fcmpge.o</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="34">
                   <c:v>dfltui.o</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="35">
                   <c:v>fflti.o</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="36">
                   <c:v>ffltui.o</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="37">
                   <c:v>entry9a.o</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="38">
                   <c:v>entry2.o</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="39">
                   <c:v>stdout.o</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="40">
                   <c:v>entry5.o</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="41">
                   <c:v>Totals</c:v>
                 </c:pt>
               </c:strCache>
@@ -447,107 +501,134 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>flash_percent!$B$3:$B$35</c:f>
+              <c:f>flash_percent!$B$3:$B$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="42"/>
                 <c:pt idx="0">
-                  <c:v>85.46077728271484</c:v>
+                  <c:v>89.39380645751953</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.563549041748047</c:v>
+                  <c:v>2.891807317733765</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.384035587310791</c:v>
+                  <c:v>2.454774856567383</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.144227504730225</c:v>
+                  <c:v>2.191685438156128</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.01404595375061</c:v>
+                  <c:v>0.4392068088054657</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.7810894250869751</c:v>
+                  <c:v>0.3631066381931305</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.760534405708313</c:v>
+                  <c:v>0.2478691935539246</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.6372045278549194</c:v>
+                  <c:v>0.2413463145494461</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.6029462218284607</c:v>
+                  <c:v>0.202209085226059</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.3768413960933685</c:v>
+                  <c:v>0.1913376301527023</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.3425830900669098</c:v>
+                  <c:v>0.1348060518503189</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.2124015092849731</c:v>
+                  <c:v>0.1195860132575035</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.137033224105835</c:v>
+                  <c:v>0.1087145581841469</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.1233299076557159</c:v>
+                  <c:v>0.1065402701497078</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.1233299076557159</c:v>
+                  <c:v>0.06740302592515945</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.1233299076557159</c:v>
+                  <c:v>0.05435727909207344</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.1233299076557159</c:v>
+                  <c:v>0.05435727909207344</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.1233299076557159</c:v>
+                  <c:v>0.05218298733234406</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.1096265837550163</c:v>
+                  <c:v>0.05218298733234406</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.1027749255299568</c:v>
+                  <c:v>0.04783440753817558</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.1027749255299568</c:v>
+                  <c:v>0.04348582401871681</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.09592325985431671</c:v>
+                  <c:v>0.04131153225898743</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.09592325985431671</c:v>
+                  <c:v>0.03913724049925804</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.09592325985431671</c:v>
+                  <c:v>0.03913724049925804</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.09592325985431671</c:v>
+                  <c:v>0.03913724049925804</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.0890716016292572</c:v>
+                  <c:v>0.03913724049925804</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.06166495382785797</c:v>
+                  <c:v>0.03696294873952866</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.03425830602645874</c:v>
+                  <c:v>0.03478866070508957</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.02740664593875408</c:v>
+                  <c:v>0.03261436894536018</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.02740664593875408</c:v>
+                  <c:v>0.03261436894536018</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.01370332296937704</c:v>
+                  <c:v>0.0304400771856308</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.01370332296937704</c:v>
+                  <c:v>0.0304400771856308</c:v>
                 </c:pt>
                 <c:pt idx="32">
+                  <c:v>0.0304400771856308</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.0304400771856308</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.02826578542590141</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.01956862024962902</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.0108714560046792</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.008697165176272392</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.008697165176272392</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.004348582588136196</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.004348582588136196</c:v>
+                </c:pt>
+                <c:pt idx="41">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -652,8 +733,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H35" totalsRowCount="1">
-  <autoFilter ref="A2:H34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H44" totalsRowCount="1">
+  <autoFilter ref="A2:H43"/>
   <tableColumns count="8">
     <tableColumn id="1" name="File_name" totalsRowLabel="Totals"/>
     <tableColumn id="2" name="ram_percent" totalsRowFunction="sum"/>
@@ -669,8 +750,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:H35" totalsRowCount="1">
-  <autoFilter ref="A2:H34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:H44" totalsRowCount="1">
+  <autoFilter ref="A2:H43"/>
   <tableColumns count="8">
     <tableColumn id="1" name="File_name" totalsRowLabel="Totals"/>
     <tableColumn id="2" name="flash_percent" totalsRowFunction="sum"/>
@@ -970,7 +1051,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -986,28 +1067,28 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1015,25 +1096,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>85.74585723876953</v>
+        <v>83.91521453857422</v>
       </c>
       <c r="C3" s="1">
-        <v>6208</v>
+        <v>5384</v>
       </c>
       <c r="D3" s="1">
-        <v>24946</v>
+        <v>82228</v>
       </c>
       <c r="E3" s="1">
-        <v>24788</v>
+        <v>81978</v>
       </c>
       <c r="F3" s="1">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="G3" s="1">
-        <v>92</v>
+        <v>144</v>
       </c>
       <c r="H3" s="1">
-        <v>6116</v>
+        <v>5240</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1041,7 +1122,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>14.14364624023438</v>
+        <v>15.9601001739502</v>
       </c>
       <c r="C4" s="1">
         <v>1024</v>
@@ -1067,16 +1148,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>0.05524861812591553</v>
+        <v>0.06234414130449295</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
       </c>
       <c r="D5" s="1">
-        <v>296</v>
+        <v>2660</v>
       </c>
       <c r="E5" s="1">
-        <v>292</v>
+        <v>2656</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -1093,7 +1174,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>0.05524861812591553</v>
+        <v>0.06234414130449295</v>
       </c>
       <c r="C6" s="1">
         <v>4</v>
@@ -1114,35 +1195,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
-      <c r="A35" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35">
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44">
         <f>SUBTOTAL(109,[ram_percent])</f>
         <v>0</v>
       </c>
-      <c r="C35">
+      <c r="C44">
         <f>SUBTOTAL(109,[ram])</f>
         <v>0</v>
       </c>
-      <c r="D35">
+      <c r="D44">
         <f>SUBTOTAL(109,[flash])</f>
         <v>0</v>
       </c>
-      <c r="E35">
+      <c r="E44">
         <f>SUBTOTAL(109,[Code])</f>
         <v>0</v>
       </c>
-      <c r="F35">
+      <c r="F44">
         <f>SUBTOTAL(109,[RO_data])</f>
         <v>0</v>
       </c>
-      <c r="G35">
+      <c r="G44">
         <f>SUBTOTAL(109,[RW_data])</f>
         <v>0</v>
       </c>
-      <c r="H35">
+      <c r="H44">
         <f>SUBTOTAL(109,[ZI_data])</f>
         <v>0</v>
       </c>
@@ -1158,7 +1239,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1174,28 +1255,28 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1203,48 +1284,48 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>85.46077728271484</v>
+        <v>89.39380645751953</v>
       </c>
       <c r="C3" s="1">
-        <v>24946</v>
+        <v>82228</v>
       </c>
       <c r="D3" s="1">
-        <v>6208</v>
+        <v>5384</v>
       </c>
       <c r="E3" s="1">
-        <v>24788</v>
+        <v>81978</v>
       </c>
       <c r="F3" s="1">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="G3" s="1">
-        <v>92</v>
+        <v>144</v>
       </c>
       <c r="H3" s="1">
-        <v>6116</v>
+        <v>5240</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>5.563549041748047</v>
+        <v>2.891807317733765</v>
       </c>
       <c r="C4" s="1">
-        <v>1624</v>
+        <v>2660</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E4" s="1">
-        <v>1624</v>
+        <v>2656</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
       </c>
       <c r="G4" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
@@ -1252,28 +1333,28 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>1.384035587310791</v>
+        <v>2.454774856567383</v>
       </c>
       <c r="C5" s="1">
-        <v>404</v>
+        <v>2258</v>
       </c>
       <c r="D5" s="1">
-        <v>1024</v>
+        <v>0</v>
       </c>
       <c r="E5" s="1">
-        <v>36</v>
+        <v>2258</v>
       </c>
       <c r="F5" s="1">
-        <v>368</v>
+        <v>0</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
       </c>
       <c r="H5" s="1">
-        <v>1024</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1281,16 +1362,16 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>1.144227504730225</v>
+        <v>2.191685438156128</v>
       </c>
       <c r="C6" s="1">
-        <v>334</v>
+        <v>2016</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>334</v>
+        <v>2016</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
@@ -1304,28 +1385,28 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" s="2">
-        <v>1.01404595375061</v>
+        <v>0.4392068088054657</v>
       </c>
       <c r="C7" s="1">
-        <v>296</v>
+        <v>404</v>
       </c>
       <c r="D7" s="1">
-        <v>4</v>
+        <v>1024</v>
       </c>
       <c r="E7" s="1">
-        <v>292</v>
+        <v>36</v>
       </c>
       <c r="F7" s="1">
-        <v>0</v>
+        <v>368</v>
       </c>
       <c r="G7" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1">
-        <v>0</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1333,16 +1414,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>0.7810894250869751</v>
+        <v>0.3631066381931305</v>
       </c>
       <c r="C8" s="1">
-        <v>228</v>
+        <v>334</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
       </c>
       <c r="E8" s="1">
-        <v>228</v>
+        <v>334</v>
       </c>
       <c r="F8" s="1">
         <v>0</v>
@@ -1359,16 +1440,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>0.760534405708313</v>
+        <v>0.2478691935539246</v>
       </c>
       <c r="C9" s="1">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
       </c>
       <c r="E9" s="1">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
@@ -1385,16 +1466,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>0.6372045278549194</v>
+        <v>0.2413463145494461</v>
       </c>
       <c r="C10" s="1">
-        <v>186</v>
+        <v>222</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
       </c>
       <c r="E10" s="1">
-        <v>186</v>
+        <v>222</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
@@ -1411,16 +1492,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>0.6029462218284607</v>
+        <v>0.202209085226059</v>
       </c>
       <c r="C11" s="1">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
       </c>
       <c r="E11" s="1">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
@@ -1437,16 +1518,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>0.3768413960933685</v>
+        <v>0.1913376301527023</v>
       </c>
       <c r="C12" s="1">
-        <v>110</v>
+        <v>176</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
       </c>
       <c r="E12" s="1">
-        <v>110</v>
+        <v>176</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
@@ -1463,16 +1544,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>0.3425830900669098</v>
+        <v>0.1348060518503189</v>
       </c>
       <c r="C13" s="1">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
       </c>
       <c r="E13" s="1">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
@@ -1489,16 +1570,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>0.2124015092849731</v>
+        <v>0.1195860132575035</v>
       </c>
       <c r="C14" s="1">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
@@ -1515,16 +1596,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>0.137033224105835</v>
+        <v>0.1087145581841469</v>
       </c>
       <c r="C15" s="1">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
       </c>
       <c r="E15" s="1">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
@@ -1541,16 +1622,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>0.1233299076557159</v>
+        <v>0.1065402701497078</v>
       </c>
       <c r="C16" s="1">
-        <v>36</v>
+        <v>98</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>36</v>
+        <v>98</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
@@ -1567,16 +1648,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>0.1233299076557159</v>
+        <v>0.06740302592515945</v>
       </c>
       <c r="C17" s="1">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
       </c>
       <c r="E17" s="1">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
@@ -1593,16 +1674,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>0.1233299076557159</v>
+        <v>0.05435727909207344</v>
       </c>
       <c r="C18" s="1">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
       </c>
       <c r="E18" s="1">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="F18" s="1">
         <v>0</v>
@@ -1619,16 +1700,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="2">
-        <v>0.1233299076557159</v>
+        <v>0.05435727909207344</v>
       </c>
       <c r="C19" s="1">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
       </c>
       <c r="E19" s="1">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
@@ -1645,16 +1726,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>0.1233299076557159</v>
+        <v>0.05218298733234406</v>
       </c>
       <c r="C20" s="1">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D20" s="1">
         <v>0</v>
       </c>
       <c r="E20" s="1">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="F20" s="1">
         <v>0</v>
@@ -1671,16 +1752,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>0.1096265837550163</v>
+        <v>0.05218298733234406</v>
       </c>
       <c r="C21" s="1">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D21" s="1">
         <v>0</v>
       </c>
       <c r="E21" s="1">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
@@ -1697,16 +1778,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>0.1027749255299568</v>
+        <v>0.04783440753817558</v>
       </c>
       <c r="C22" s="1">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
       </c>
       <c r="E22" s="1">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="F22" s="1">
         <v>0</v>
@@ -1723,16 +1804,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="2">
-        <v>0.1027749255299568</v>
+        <v>0.04348582401871681</v>
       </c>
       <c r="C23" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
       </c>
       <c r="E23" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F23" s="1">
         <v>0</v>
@@ -1749,16 +1830,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="2">
-        <v>0.09592325985431671</v>
+        <v>0.04131153225898743</v>
       </c>
       <c r="C24" s="1">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
       </c>
       <c r="E24" s="1">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="F24" s="1">
         <v>0</v>
@@ -1775,16 +1856,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="2">
-        <v>0.09592325985431671</v>
+        <v>0.03913724049925804</v>
       </c>
       <c r="C25" s="1">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D25" s="1">
         <v>0</v>
       </c>
       <c r="E25" s="1">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="F25" s="1">
         <v>0</v>
@@ -1801,16 +1882,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="2">
-        <v>0.09592325985431671</v>
+        <v>0.03913724049925804</v>
       </c>
       <c r="C26" s="1">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
       </c>
       <c r="E26" s="1">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="F26" s="1">
         <v>0</v>
@@ -1827,16 +1908,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="2">
-        <v>0.09592325985431671</v>
+        <v>0.03913724049925804</v>
       </c>
       <c r="C27" s="1">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D27" s="1">
         <v>0</v>
       </c>
       <c r="E27" s="1">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="F27" s="1">
         <v>0</v>
@@ -1853,16 +1934,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="2">
-        <v>0.0890716016292572</v>
+        <v>0.03913724049925804</v>
       </c>
       <c r="C28" s="1">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="D28" s="1">
         <v>0</v>
       </c>
       <c r="E28" s="1">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="F28" s="1">
         <v>0</v>
@@ -1879,16 +1960,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="2">
-        <v>0.06166495382785797</v>
+        <v>0.03696294873952866</v>
       </c>
       <c r="C29" s="1">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D29" s="1">
         <v>0</v>
       </c>
       <c r="E29" s="1">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
@@ -1905,16 +1986,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="2">
-        <v>0.03425830602645874</v>
+        <v>0.03478866070508957</v>
       </c>
       <c r="C30" s="1">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
       </c>
       <c r="E30" s="1">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="F30" s="1">
         <v>0</v>
@@ -1931,16 +2012,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="2">
-        <v>0.02740664593875408</v>
+        <v>0.03261436894536018</v>
       </c>
       <c r="C31" s="1">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="D31" s="1">
         <v>0</v>
       </c>
       <c r="E31" s="1">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="F31" s="1">
         <v>0</v>
@@ -1957,16 +2038,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="2">
-        <v>0.02740664593875408</v>
+        <v>0.03261436894536018</v>
       </c>
       <c r="C32" s="1">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="D32" s="1">
         <v>0</v>
       </c>
       <c r="E32" s="1">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="F32" s="1">
         <v>0</v>
@@ -1980,25 +2061,25 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B33" s="2">
-        <v>0.01370332296937704</v>
+        <v>0.0304400771856308</v>
       </c>
       <c r="C33" s="1">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="D33" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E33" s="1">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F33" s="1">
         <v>0</v>
       </c>
       <c r="G33" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H33" s="1">
         <v>0</v>
@@ -2006,59 +2087,293 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" s="2">
-        <v>0.01370332296937704</v>
+        <v>0.0304400771856308</v>
       </c>
       <c r="C34" s="1">
+        <v>28</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
+        <v>28</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0.0304400771856308</v>
+      </c>
+      <c r="C35" s="1">
+        <v>28</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1">
+        <v>28</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2">
+        <v>0.0304400771856308</v>
+      </c>
+      <c r="C36" s="1">
+        <v>28</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1">
+        <v>28</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2">
+        <v>0.02826578542590141</v>
+      </c>
+      <c r="C37" s="1">
+        <v>26</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0</v>
+      </c>
+      <c r="E37" s="1">
+        <v>26</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0.01956862024962902</v>
+      </c>
+      <c r="C38" s="1">
+        <v>18</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0</v>
+      </c>
+      <c r="E38" s="1">
+        <v>18</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0</v>
+      </c>
+      <c r="H38" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2">
+        <v>0.0108714560046792</v>
+      </c>
+      <c r="C39" s="1">
+        <v>10</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1">
+        <v>10</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0</v>
+      </c>
+      <c r="G39" s="1">
+        <v>0</v>
+      </c>
+      <c r="H39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2">
+        <v>0.008697165176272392</v>
+      </c>
+      <c r="C40" s="1">
+        <v>8</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1">
+        <v>8</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0</v>
+      </c>
+      <c r="H40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2">
+        <v>0.008697165176272392</v>
+      </c>
+      <c r="C41" s="1">
+        <v>8</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1">
+        <v>8</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="1">
-        <v>0</v>
-      </c>
-      <c r="E34" s="1">
+      <c r="B42" s="2">
+        <v>0.004348582588136196</v>
+      </c>
+      <c r="C42" s="1">
         <v>4</v>
       </c>
-      <c r="F34" s="1">
-        <v>0</v>
-      </c>
-      <c r="G34" s="1">
-        <v>0</v>
-      </c>
-      <c r="H34" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35">
+      <c r="D42" s="1">
+        <v>4</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0</v>
+      </c>
+      <c r="G42" s="1">
+        <v>4</v>
+      </c>
+      <c r="H42" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="2">
+        <v>0.004348582588136196</v>
+      </c>
+      <c r="C43" s="1">
+        <v>4</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0</v>
+      </c>
+      <c r="E43" s="1">
+        <v>4</v>
+      </c>
+      <c r="F43" s="1">
+        <v>0</v>
+      </c>
+      <c r="G43" s="1">
+        <v>0</v>
+      </c>
+      <c r="H43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44">
         <f>SUBTOTAL(109,[flash_percent])</f>
         <v>0</v>
       </c>
-      <c r="C35">
+      <c r="C44">
         <f>SUBTOTAL(109,[flash])</f>
         <v>0</v>
       </c>
-      <c r="D35">
+      <c r="D44">
         <f>SUBTOTAL(109,[ram])</f>
         <v>0</v>
       </c>
-      <c r="E35">
+      <c r="E44">
         <f>SUBTOTAL(109,[Code])</f>
         <v>0</v>
       </c>
-      <c r="F35">
+      <c r="F44">
         <f>SUBTOTAL(109,[RO_data])</f>
         <v>0</v>
       </c>
-      <c r="G35">
+      <c r="G44">
         <f>SUBTOTAL(109,[RW_data])</f>
         <v>0</v>
       </c>
-      <c r="H35">
+      <c r="H44">
         <f>SUBTOTAL(109,[ZI_data])</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
fix curve error, add wind bar and temp bar adjust the temp and wind
</commit_message>
<xml_diff>
--- a/app/project/MDK_V5/AT32F415RBT7_WorkBench_analysis.xlsx
+++ b/app/project/MDK_V5/AT32F415RBT7_WorkBench_analysis.xlsx
@@ -15,12 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
   <si>
     <t>AT32F415RBT7_WorkBench</t>
   </si>
   <si>
-    <t>lto-llvm-5b4722.o</t>
+    <t>lto-llvm-7975cf.o</t>
   </si>
   <si>
     <t>startup_at32f415.o</t>
@@ -32,12 +32,12 @@
     <t>stdout.o</t>
   </si>
   <si>
-    <t>printfa.o</t>
-  </si>
-  <si>
     <t>mf_w.l</t>
   </si>
   <si>
+    <t>printf6.o</t>
+  </si>
+  <si>
     <t>dadd.o</t>
   </si>
   <si>
@@ -62,9 +62,6 @@
     <t>fmul.o</t>
   </si>
   <si>
-    <t>uldiv.o</t>
-  </si>
-  <si>
     <t>dfixi.o</t>
   </si>
   <si>
@@ -74,12 +71,6 @@
     <t>dfixui.o</t>
   </si>
   <si>
-    <t>dfixul.o</t>
-  </si>
-  <si>
-    <t>cdrcmple.o</t>
-  </si>
-  <si>
     <t>uidiv.o</t>
   </si>
   <si>
@@ -87,6 +78,9 @@
   </si>
   <si>
     <t>f2d.o</t>
+  </si>
+  <si>
+    <t>puts.o</t>
   </si>
   <si>
     <t>memseta.o</t>
@@ -260,11 +254,11 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>ram_percent!$A$3:$A$44</c:f>
+              <c:f>ram_percent!$A$3:$A$42</c:f>
               <c:strCache>
-                <c:ptCount val="42"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>lto-llvm-5b4722.o</c:v>
+                  <c:v>lto-llvm-7975cf.o</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>startup_at32f415.o</c:v>
@@ -275,7 +269,7 @@
                 <c:pt idx="3">
                   <c:v>stdout.o</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="39">
                   <c:v>Totals</c:v>
                 </c:pt>
               </c:strCache>
@@ -283,23 +277,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ram_percent!$B$3:$B$44</c:f>
+              <c:f>ram_percent!$B$3:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>83.91521453857422</c:v>
+                  <c:v>83.51437377929688</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.9601001739502</c:v>
+                  <c:v>16.35782814025879</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.06234414130449295</c:v>
+                  <c:v>0.0638977661728859</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.06234414130449295</c:v>
-                </c:pt>
-                <c:pt idx="41">
+                  <c:v>0.0638977661728859</c:v>
+                </c:pt>
+                <c:pt idx="39">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -367,20 +361,20 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>flash_percent!$A$3:$A$44</c:f>
+              <c:f>flash_percent!$A$3:$A$42</c:f>
               <c:strCache>
-                <c:ptCount val="42"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>lto-llvm-5b4722.o</c:v>
+                  <c:v>lto-llvm-7975cf.o</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>mf_w.l</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>mc_w.l</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>printfa.o</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>mf_w.l</c:v>
+                  <c:v>printf6.o</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>startup_at32f415.o</c:v>
@@ -410,90 +404,84 @@
                   <c:v>fmul.o</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>uldiv.o</c:v>
+                  <c:v>dfixi.o</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>dfixi.o</c:v>
+                  <c:v>ffixi.o</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>ffixi.o</c:v>
+                  <c:v>dfixui.o</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>dfixui.o</c:v>
+                  <c:v>uidiv.o</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>dfixul.o</c:v>
+                  <c:v>ffixui.o</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>cdrcmple.o</c:v>
+                  <c:v>f2d.o</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>uidiv.o</c:v>
+                  <c:v>puts.o</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>ffixui.o</c:v>
+                  <c:v>memseta.o</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>f2d.o</c:v>
+                  <c:v>memcpya.o</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>memseta.o</c:v>
+                  <c:v>llsshr.o</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>memcpya.o</c:v>
+                  <c:v>init.o</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>llsshr.o</c:v>
+                  <c:v>dflti.o</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>init.o</c:v>
+                  <c:v>llushr.o</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>dflti.o</c:v>
+                  <c:v>llshl.o</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>llushr.o</c:v>
+                  <c:v>handlers.o</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>llshl.o</c:v>
+                  <c:v>fcmplt.o</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>handlers.o</c:v>
+                  <c:v>fcmple.o</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>fcmplt.o</c:v>
+                  <c:v>fcmpgt.o</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>fcmple.o</c:v>
+                  <c:v>fcmpge.o</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>fcmpgt.o</c:v>
+                  <c:v>dfltui.o</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>fcmpge.o</c:v>
+                  <c:v>fflti.o</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>dfltui.o</c:v>
+                  <c:v>ffltui.o</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>fflti.o</c:v>
+                  <c:v>entry9a.o</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>ffltui.o</c:v>
+                  <c:v>entry2.o</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>entry9a.o</c:v>
+                  <c:v>stdout.o</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>entry2.o</c:v>
+                  <c:v>entry5.o</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>stdout.o</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>entry5.o</c:v>
-                </c:pt>
-                <c:pt idx="41">
                   <c:v>Totals</c:v>
                 </c:pt>
               </c:strCache>
@@ -501,134 +489,128 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>flash_percent!$B$3:$B$44</c:f>
+              <c:f>flash_percent!$B$3:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>89.39380645751953</c:v>
+                  <c:v>82.97262573242188</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.891807317733765</c:v>
+                  <c:v>4.911742210388184</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.454774856567383</c:v>
+                  <c:v>3.085187911987305</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.191685438156128</c:v>
+                  <c:v>2.215400457382202</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.4392068088054657</c:v>
+                  <c:v>1.033512353897095</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.3631066381931305</c:v>
+                  <c:v>0.8544384837150574</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.2478691935539246</c:v>
+                  <c:v>0.5832693576812744</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.2413463145494461</c:v>
+                  <c:v>0.5679202079772949</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.202209085226059</c:v>
+                  <c:v>0.4758250117301941</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1913376301527023</c:v>
+                  <c:v>0.4502430260181427</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1348060518503189</c:v>
+                  <c:v>0.317216694355011</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.1195860132575035</c:v>
+                  <c:v>0.2814019024372101</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.1087145581841469</c:v>
+                  <c:v>0.2558199167251587</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.1065402701497078</c:v>
+                  <c:v>0.1586083471775055</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.06740302592515945</c:v>
+                  <c:v>0.1279099583625794</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.05435727909207344</c:v>
+                  <c:v>0.1279099583625794</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.05435727909207344</c:v>
+                  <c:v>0.1125607565045357</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.05218298733234406</c:v>
+                  <c:v>0.1023279577493668</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.05218298733234406</c:v>
+                  <c:v>0.0972115620970726</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.04783440753817558</c:v>
+                  <c:v>0.09209516644477844</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.04348582401871681</c:v>
+                  <c:v>0.09209516644477844</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.04131153225898743</c:v>
+                  <c:v>0.09209516644477844</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.03913724049925804</c:v>
+                  <c:v>0.09209516644477844</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.03913724049925804</c:v>
+                  <c:v>0.09209516644477844</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.03913724049925804</c:v>
+                  <c:v>0.08697876334190369</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.03913724049925804</c:v>
+                  <c:v>0.08186236768960953</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.03696294873952866</c:v>
+                  <c:v>0.07674597203731537</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.03478866070508957</c:v>
+                  <c:v>0.07674597203731537</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.03261436894536018</c:v>
+                  <c:v>0.07162957638502121</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.03261436894536018</c:v>
+                  <c:v>0.07162957638502121</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.0304400771856308</c:v>
+                  <c:v>0.07162957638502121</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.0304400771856308</c:v>
+                  <c:v>0.07162957638502121</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.0304400771856308</c:v>
+                  <c:v>0.06651317328214645</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.0304400771856308</c:v>
+                  <c:v>0.04604758322238922</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.02826578542590141</c:v>
+                  <c:v>0.02558198943734169</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.01956862024962902</c:v>
+                  <c:v>0.02046559192240238</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.0108714560046792</c:v>
+                  <c:v>0.02046559192240238</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.008697165176272392</c:v>
+                  <c:v>0.01023279596120119</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.008697165176272392</c:v>
+                  <c:v>0.01023279596120119</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.004348582588136196</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.004348582588136196</c:v>
-                </c:pt>
-                <c:pt idx="41">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -733,8 +715,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H44" totalsRowCount="1">
-  <autoFilter ref="A2:H43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H42" totalsRowCount="1">
+  <autoFilter ref="A2:H41"/>
   <tableColumns count="8">
     <tableColumn id="1" name="File_name" totalsRowLabel="Totals"/>
     <tableColumn id="2" name="ram_percent" totalsRowFunction="sum"/>
@@ -750,8 +732,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:H44" totalsRowCount="1">
-  <autoFilter ref="A2:H43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:H42" totalsRowCount="1">
+  <autoFilter ref="A2:H41"/>
   <tableColumns count="8">
     <tableColumn id="1" name="File_name" totalsRowLabel="Totals"/>
     <tableColumn id="2" name="flash_percent" totalsRowFunction="sum"/>
@@ -1051,7 +1033,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1067,28 +1049,28 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
         <v>42</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>45</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>46</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>47</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>48</v>
-      </c>
-      <c r="G2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1096,25 +1078,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>83.91521453857422</v>
+        <v>83.51437377929688</v>
       </c>
       <c r="C3" s="1">
-        <v>5384</v>
+        <v>5228</v>
       </c>
       <c r="D3" s="1">
-        <v>82228</v>
+        <v>32434</v>
       </c>
       <c r="E3" s="1">
-        <v>81978</v>
+        <v>32244</v>
       </c>
       <c r="F3" s="1">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="G3" s="1">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="H3" s="1">
-        <v>5240</v>
+        <v>5104</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1122,7 +1104,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>15.9601001739502</v>
+        <v>16.35782814025879</v>
       </c>
       <c r="C4" s="1">
         <v>1024</v>
@@ -1148,16 +1130,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>0.06234414130449295</v>
+        <v>0.0638977661728859</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
       </c>
       <c r="D5" s="1">
-        <v>2660</v>
+        <v>1206</v>
       </c>
       <c r="E5" s="1">
-        <v>2656</v>
+        <v>1202</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -1174,7 +1156,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>0.06234414130449295</v>
+        <v>0.0638977661728859</v>
       </c>
       <c r="C6" s="1">
         <v>4</v>
@@ -1195,35 +1177,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
-      <c r="A44" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44">
+    <row r="42" spans="1:8">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42">
         <f>SUBTOTAL(109,[ram_percent])</f>
         <v>0</v>
       </c>
-      <c r="C44">
+      <c r="C42">
         <f>SUBTOTAL(109,[ram])</f>
         <v>0</v>
       </c>
-      <c r="D44">
+      <c r="D42">
         <f>SUBTOTAL(109,[flash])</f>
         <v>0</v>
       </c>
-      <c r="E44">
+      <c r="E42">
         <f>SUBTOTAL(109,[Code])</f>
         <v>0</v>
       </c>
-      <c r="F44">
+      <c r="F42">
         <f>SUBTOTAL(109,[RO_data])</f>
         <v>0</v>
       </c>
-      <c r="G44">
+      <c r="G42">
         <f>SUBTOTAL(109,[RW_data])</f>
         <v>0</v>
       </c>
-      <c r="H44">
+      <c r="H42">
         <f>SUBTOTAL(109,[ZI_data])</f>
         <v>0</v>
       </c>
@@ -1239,7 +1221,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1255,28 +1237,28 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
         <v>46</v>
       </c>
-      <c r="D2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>47</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>48</v>
-      </c>
-      <c r="G2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1284,48 +1266,48 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>89.39380645751953</v>
+        <v>82.97262573242188</v>
       </c>
       <c r="C3" s="1">
-        <v>82228</v>
+        <v>32434</v>
       </c>
       <c r="D3" s="1">
-        <v>5384</v>
+        <v>5228</v>
       </c>
       <c r="E3" s="1">
-        <v>81978</v>
+        <v>32244</v>
       </c>
       <c r="F3" s="1">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="G3" s="1">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="H3" s="1">
-        <v>5240</v>
+        <v>5104</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2">
-        <v>2.891807317733765</v>
+        <v>4.911742210388184</v>
       </c>
       <c r="C4" s="1">
-        <v>2660</v>
+        <v>1920</v>
       </c>
       <c r="D4" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1">
-        <v>2656</v>
+        <v>1920</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
       </c>
       <c r="G4" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
@@ -1333,25 +1315,25 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>2.454774856567383</v>
+        <v>3.085187911987305</v>
       </c>
       <c r="C5" s="1">
-        <v>2258</v>
+        <v>1206</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E5" s="1">
-        <v>2258</v>
+        <v>1202</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
       </c>
       <c r="G5" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H5" s="1">
         <v>0</v>
@@ -1362,16 +1344,16 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>2.191685438156128</v>
+        <v>2.215400457382202</v>
       </c>
       <c r="C6" s="1">
-        <v>2016</v>
+        <v>866</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>2016</v>
+        <v>866</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
@@ -1388,7 +1370,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="2">
-        <v>0.4392068088054657</v>
+        <v>1.033512353897095</v>
       </c>
       <c r="C7" s="1">
         <v>404</v>
@@ -1414,7 +1396,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>0.3631066381931305</v>
+        <v>0.8544384837150574</v>
       </c>
       <c r="C8" s="1">
         <v>334</v>
@@ -1440,7 +1422,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>0.2478691935539246</v>
+        <v>0.5832693576812744</v>
       </c>
       <c r="C9" s="1">
         <v>228</v>
@@ -1466,7 +1448,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>0.2413463145494461</v>
+        <v>0.5679202079772949</v>
       </c>
       <c r="C10" s="1">
         <v>222</v>
@@ -1492,7 +1474,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>0.202209085226059</v>
+        <v>0.4758250117301941</v>
       </c>
       <c r="C11" s="1">
         <v>186</v>
@@ -1518,7 +1500,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>0.1913376301527023</v>
+        <v>0.4502430260181427</v>
       </c>
       <c r="C12" s="1">
         <v>176</v>
@@ -1544,7 +1526,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>0.1348060518503189</v>
+        <v>0.317216694355011</v>
       </c>
       <c r="C13" s="1">
         <v>124</v>
@@ -1570,7 +1552,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>0.1195860132575035</v>
+        <v>0.2814019024372101</v>
       </c>
       <c r="C14" s="1">
         <v>110</v>
@@ -1596,7 +1578,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>0.1087145581841469</v>
+        <v>0.2558199167251587</v>
       </c>
       <c r="C15" s="1">
         <v>100</v>
@@ -1622,16 +1604,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>0.1065402701497078</v>
+        <v>0.1586083471775055</v>
       </c>
       <c r="C16" s="1">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
@@ -1648,16 +1630,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>0.06740302592515945</v>
+        <v>0.1279099583625794</v>
       </c>
       <c r="C17" s="1">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
       </c>
       <c r="E17" s="1">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
@@ -1674,7 +1656,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>0.05435727909207344</v>
+        <v>0.1279099583625794</v>
       </c>
       <c r="C18" s="1">
         <v>50</v>
@@ -1700,16 +1682,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="2">
-        <v>0.05435727909207344</v>
+        <v>0.1125607565045357</v>
       </c>
       <c r="C19" s="1">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
       </c>
       <c r="E19" s="1">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
@@ -1726,16 +1708,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>0.05218298733234406</v>
+        <v>0.1023279577493668</v>
       </c>
       <c r="C20" s="1">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D20" s="1">
         <v>0</v>
       </c>
       <c r="E20" s="1">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F20" s="1">
         <v>0</v>
@@ -1752,16 +1734,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>0.05218298733234406</v>
+        <v>0.0972115620970726</v>
       </c>
       <c r="C21" s="1">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D21" s="1">
         <v>0</v>
       </c>
       <c r="E21" s="1">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
@@ -1778,16 +1760,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>0.04783440753817558</v>
+        <v>0.09209516644477844</v>
       </c>
       <c r="C22" s="1">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
       </c>
       <c r="E22" s="1">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F22" s="1">
         <v>0</v>
@@ -1804,16 +1786,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="2">
-        <v>0.04348582401871681</v>
+        <v>0.09209516644477844</v>
       </c>
       <c r="C23" s="1">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
       </c>
       <c r="E23" s="1">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F23" s="1">
         <v>0</v>
@@ -1830,16 +1812,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="2">
-        <v>0.04131153225898743</v>
+        <v>0.09209516644477844</v>
       </c>
       <c r="C24" s="1">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
       </c>
       <c r="E24" s="1">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F24" s="1">
         <v>0</v>
@@ -1856,7 +1838,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2">
-        <v>0.03913724049925804</v>
+        <v>0.09209516644477844</v>
       </c>
       <c r="C25" s="1">
         <v>36</v>
@@ -1882,7 +1864,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2">
-        <v>0.03913724049925804</v>
+        <v>0.09209516644477844</v>
       </c>
       <c r="C26" s="1">
         <v>36</v>
@@ -1908,16 +1890,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="2">
-        <v>0.03913724049925804</v>
+        <v>0.08697876334190369</v>
       </c>
       <c r="C27" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D27" s="1">
         <v>0</v>
       </c>
       <c r="E27" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F27" s="1">
         <v>0</v>
@@ -1934,16 +1916,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="2">
-        <v>0.03913724049925804</v>
+        <v>0.08186236768960953</v>
       </c>
       <c r="C28" s="1">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D28" s="1">
         <v>0</v>
       </c>
       <c r="E28" s="1">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F28" s="1">
         <v>0</v>
@@ -1960,16 +1942,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="2">
-        <v>0.03696294873952866</v>
+        <v>0.07674597203731537</v>
       </c>
       <c r="C29" s="1">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D29" s="1">
         <v>0</v>
       </c>
       <c r="E29" s="1">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
@@ -1986,16 +1968,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="2">
-        <v>0.03478866070508957</v>
+        <v>0.07674597203731537</v>
       </c>
       <c r="C30" s="1">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
       </c>
       <c r="E30" s="1">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F30" s="1">
         <v>0</v>
@@ -2012,16 +1994,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="2">
-        <v>0.03261436894536018</v>
+        <v>0.07162957638502121</v>
       </c>
       <c r="C31" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D31" s="1">
         <v>0</v>
       </c>
       <c r="E31" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F31" s="1">
         <v>0</v>
@@ -2038,16 +2020,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="2">
-        <v>0.03261436894536018</v>
+        <v>0.07162957638502121</v>
       </c>
       <c r="C32" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D32" s="1">
         <v>0</v>
       </c>
       <c r="E32" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F32" s="1">
         <v>0</v>
@@ -2064,7 +2046,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="2">
-        <v>0.0304400771856308</v>
+        <v>0.07162957638502121</v>
       </c>
       <c r="C33" s="1">
         <v>28</v>
@@ -2090,7 +2072,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="2">
-        <v>0.0304400771856308</v>
+        <v>0.07162957638502121</v>
       </c>
       <c r="C34" s="1">
         <v>28</v>
@@ -2116,16 +2098,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="2">
-        <v>0.0304400771856308</v>
+        <v>0.06651317328214645</v>
       </c>
       <c r="C35" s="1">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D35" s="1">
         <v>0</v>
       </c>
       <c r="E35" s="1">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F35" s="1">
         <v>0</v>
@@ -2142,16 +2124,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="2">
-        <v>0.0304400771856308</v>
+        <v>0.04604758322238922</v>
       </c>
       <c r="C36" s="1">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D36" s="1">
         <v>0</v>
       </c>
       <c r="E36" s="1">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F36" s="1">
         <v>0</v>
@@ -2168,16 +2150,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="2">
-        <v>0.02826578542590141</v>
+        <v>0.02558198943734169</v>
       </c>
       <c r="C37" s="1">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D37" s="1">
         <v>0</v>
       </c>
       <c r="E37" s="1">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="F37" s="1">
         <v>0</v>
@@ -2194,16 +2176,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="2">
-        <v>0.01956862024962902</v>
+        <v>0.02046559192240238</v>
       </c>
       <c r="C38" s="1">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D38" s="1">
         <v>0</v>
       </c>
       <c r="E38" s="1">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F38" s="1">
         <v>0</v>
@@ -2220,16 +2202,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="2">
-        <v>0.0108714560046792</v>
+        <v>0.02046559192240238</v>
       </c>
       <c r="C39" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D39" s="1">
         <v>0</v>
       </c>
       <c r="E39" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F39" s="1">
         <v>0</v>
@@ -2243,25 +2225,25 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="B40" s="2">
-        <v>0.008697165176272392</v>
+        <v>0.01023279596120119</v>
       </c>
       <c r="C40" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D40" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E40" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F40" s="1">
         <v>0</v>
       </c>
       <c r="G40" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H40" s="1">
         <v>0</v>
@@ -2269,19 +2251,19 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" s="2">
-        <v>0.008697165176272392</v>
+        <v>0.01023279596120119</v>
       </c>
       <c r="C41" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D41" s="1">
         <v>0</v>
       </c>
       <c r="E41" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F41" s="1">
         <v>0</v>
@@ -2294,86 +2276,34 @@
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="2">
-        <v>0.004348582588136196</v>
-      </c>
-      <c r="C42" s="1">
-        <v>4</v>
-      </c>
-      <c r="D42" s="1">
-        <v>4</v>
-      </c>
-      <c r="E42" s="1">
-        <v>0</v>
-      </c>
-      <c r="F42" s="1">
-        <v>0</v>
-      </c>
-      <c r="G42" s="1">
-        <v>4</v>
-      </c>
-      <c r="H42" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="1" t="s">
+      <c r="A42" t="s">
         <v>41</v>
       </c>
-      <c r="B43" s="2">
-        <v>0.004348582588136196</v>
-      </c>
-      <c r="C43" s="1">
-        <v>4</v>
-      </c>
-      <c r="D43" s="1">
-        <v>0</v>
-      </c>
-      <c r="E43" s="1">
-        <v>4</v>
-      </c>
-      <c r="F43" s="1">
-        <v>0</v>
-      </c>
-      <c r="G43" s="1">
-        <v>0</v>
-      </c>
-      <c r="H43" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44">
+      <c r="B42">
         <f>SUBTOTAL(109,[flash_percent])</f>
         <v>0</v>
       </c>
-      <c r="C44">
+      <c r="C42">
         <f>SUBTOTAL(109,[flash])</f>
         <v>0</v>
       </c>
-      <c r="D44">
+      <c r="D42">
         <f>SUBTOTAL(109,[ram])</f>
         <v>0</v>
       </c>
-      <c r="E44">
+      <c r="E42">
         <f>SUBTOTAL(109,[Code])</f>
         <v>0</v>
       </c>
-      <c r="F44">
+      <c r="F42">
         <f>SUBTOTAL(109,[RO_data])</f>
         <v>0</v>
       </c>
-      <c r="G44">
+      <c r="G42">
         <f>SUBTOTAL(109,[RW_data])</f>
         <v>0</v>
       </c>
-      <c r="H44">
+      <c r="H42">
         <f>SUBTOTAL(109,[ZI_data])</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
fix channel select state display error
</commit_message>
<xml_diff>
--- a/app/project/MDK_V5/AT32F415RBT7_WorkBench_analysis.xlsx
+++ b/app/project/MDK_V5/AT32F415RBT7_WorkBench_analysis.xlsx
@@ -20,7 +20,7 @@
     <t>AT32F415RBT7_WorkBench</t>
   </si>
   <si>
-    <t>lto-llvm-7975cf.o</t>
+    <t>lto-llvm-86ee4b.o</t>
   </si>
   <si>
     <t>startup_at32f415.o</t>
@@ -258,7 +258,7 @@
               <c:strCache>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>lto-llvm-7975cf.o</c:v>
+                  <c:v>lto-llvm-86ee4b.o</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>startup_at32f415.o</c:v>
@@ -365,7 +365,7 @@
               <c:strCache>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>lto-llvm-7975cf.o</c:v>
+                  <c:v>lto-llvm-86ee4b.o</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>mf_w.l</c:v>

</xml_diff>